<commit_message>
update codificação e tabelas
Tudo retficado e coerente
</commit_message>
<xml_diff>
--- a/Tabelas BVA.xlsx
+++ b/Tabelas BVA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunof\Desktop\Universidade\PAW\ESII--TP2.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vieir\Documents\GitHub\ESII--TP2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B10C2A8-20EC-4B36-ABB4-92F809828EC5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F92A6DE1-25B6-4196-BAF4-F503834B1A05}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10395" xr2:uid="{5BC89611-3435-46D4-BA42-03AA10355231}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10392" xr2:uid="{5BC89611-3435-46D4-BA42-03AA10355231}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="53">
   <si>
     <t>Casos de Teste</t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t>maximoFicheiros</t>
+  </si>
+  <si>
+    <t>numFiles&gt;0</t>
+  </si>
+  <si>
+    <t>numFiles&lt;=0</t>
   </si>
 </sst>
 </file>
@@ -375,22 +381,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -718,48 +724,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD84452C-D8AA-4605-BDBF-5DDB03E4E521}">
-  <dimension ref="A1:G123"/>
+  <dimension ref="A1:G120"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A89" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67:F67"/>
+      <selection activeCell="H101" sqref="H101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" customWidth="1"/>
-    <col min="6" max="6" width="42.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" customWidth="1"/>
+    <col min="6" max="6" width="42.5546875" customWidth="1"/>
     <col min="7" max="7" width="37" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" customWidth="1"/>
-    <col min="12" max="12" width="7.42578125" customWidth="1"/>
-    <col min="13" max="13" width="37.7109375" customWidth="1"/>
-    <col min="15" max="15" width="20.28515625" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" customWidth="1"/>
+    <col min="12" max="12" width="7.44140625" customWidth="1"/>
+    <col min="13" max="13" width="37.6640625" customWidth="1"/>
+    <col min="15" max="15" width="20.33203125" customWidth="1"/>
     <col min="20" max="20" width="19" customWidth="1"/>
-    <col min="21" max="21" width="15.5703125" customWidth="1"/>
-    <col min="23" max="23" width="20.7109375" customWidth="1"/>
-    <col min="26" max="26" width="12.85546875" customWidth="1"/>
-    <col min="28" max="28" width="15.85546875" customWidth="1"/>
+    <col min="21" max="21" width="15.5546875" customWidth="1"/>
+    <col min="23" max="23" width="20.6640625" customWidth="1"/>
+    <col min="26" max="26" width="12.88671875" customWidth="1"/>
+    <col min="28" max="28" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -770,106 +776,106 @@
       <c r="F3" s="5"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>1</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>2</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
       <c r="E7" s="10"/>
       <c r="F7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="19"/>
       <c r="E8" s="10"/>
       <c r="G8" s="10"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>1</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="19"/>
       <c r="E9" s="10"/>
       <c r="F9" s="4" t="s">
         <v>12</v>
       </c>
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>2</v>
       </c>
       <c r="B10" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="19"/>
       <c r="E10" s="10"/>
       <c r="F10" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="10"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -879,104 +885,104 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>1</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>2</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G17" s="10"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
       <c r="E18" s="10"/>
       <c r="F18" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G18" s="10"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B19" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="19"/>
       <c r="E19" s="10"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>1</v>
       </c>
       <c r="B20" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="19"/>
       <c r="E20" s="10"/>
       <c r="F20" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G20" s="10"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>2</v>
       </c>
       <c r="B21" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="19"/>
       <c r="E21" s="10"/>
       <c r="F21" s="4" t="s">
         <v>22</v>
       </c>
       <c r="G21" s="10"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G22" s="10"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
       <c r="G23" s="10"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -985,7 +991,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="10"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>1</v>
       </c>
@@ -996,33 +1002,33 @@
       <c r="F25" s="2"/>
       <c r="G25" s="10"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>1</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>2</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
       <c r="G27" s="10"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1031,7 +1037,7 @@
       <c r="F28" s="1"/>
       <c r="G28" s="10"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>0</v>
       </c>
@@ -1046,48 +1052,48 @@
       </c>
       <c r="G29" s="10"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="19"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="10"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>1</v>
       </c>
       <c r="B31" s="17">
         <v>1</v>
       </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="19"/>
       <c r="E31" s="14"/>
       <c r="F31" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G31" s="10"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>2</v>
       </c>
       <c r="B32" s="17">
         <v>0</v>
       </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="19"/>
       <c r="E32" s="14"/>
       <c r="F32" s="4" t="s">
         <v>22</v>
       </c>
       <c r="G32" s="11"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1095,19 +1101,19 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B34" s="20" t="s">
+      <c r="B34" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1115,7 +1121,7 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>1</v>
       </c>
@@ -1125,31 +1131,31 @@
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
         <v>1</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="B37" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
         <v>2</v>
       </c>
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1157,7 +1163,7 @@
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>0</v>
       </c>
@@ -1171,57 +1177,57 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C41" s="19"/>
-      <c r="D41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="19"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="6">
         <v>1</v>
       </c>
       <c r="B42" s="17">
         <v>1</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="18"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="19"/>
       <c r="E42" s="14"/>
       <c r="F42" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="6">
         <v>2</v>
       </c>
       <c r="B43" s="17">
         <v>0</v>
       </c>
-      <c r="C43" s="19"/>
-      <c r="D43" s="18"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="19"/>
       <c r="E43" s="14"/>
       <c r="F43" s="4">
         <v>-1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="16" t="s">
+      <c r="B46" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C46" s="16"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="16"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1229,7 +1235,7 @@
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>1</v>
       </c>
@@ -1239,55 +1245,55 @@
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="6">
         <v>1</v>
       </c>
-      <c r="B49" s="15" t="s">
+      <c r="B49" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="15"/>
-      <c r="F49" s="15"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C49" s="16"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="6">
         <v>2</v>
       </c>
-      <c r="B50" s="15" t="s">
+      <c r="B50" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C50" s="15"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="15"/>
-      <c r="F50" s="15"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C50" s="16"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="6">
         <v>3</v>
       </c>
-      <c r="B51" s="15" t="s">
+      <c r="B51" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C51" s="15"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="15"/>
-      <c r="F51" s="15"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C51" s="16"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="16"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="6">
         <v>4</v>
       </c>
-      <c r="B52" s="15" t="s">
+      <c r="B52" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C52" s="15"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="15"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C52" s="16"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1295,7 +1301,7 @@
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>0</v>
       </c>
@@ -1309,7 +1315,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="8" t="s">
         <v>26</v>
@@ -1323,7 +1329,7 @@
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="6">
         <v>1</v>
       </c>
@@ -1341,7 +1347,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="6">
         <v>2</v>
       </c>
@@ -1359,7 +1365,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="6">
         <v>3</v>
       </c>
@@ -1377,7 +1383,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="6">
         <v>4</v>
       </c>
@@ -1395,7 +1401,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="6">
         <v>5</v>
       </c>
@@ -1413,7 +1419,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="6">
         <v>6</v>
       </c>
@@ -1431,7 +1437,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1439,7 +1445,7 @@
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1447,19 +1453,19 @@
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B64" s="16" t="s">
+      <c r="B64" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C64" s="16"/>
-      <c r="D64" s="16"/>
-      <c r="E64" s="16"/>
-      <c r="F64" s="16"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C64" s="20"/>
+      <c r="D64" s="20"/>
+      <c r="E64" s="20"/>
+      <c r="F64" s="20"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1467,7 +1473,7 @@
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>1</v>
       </c>
@@ -1477,55 +1483,55 @@
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="6">
         <v>1</v>
       </c>
-      <c r="B67" s="15" t="s">
+      <c r="B67" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C67" s="15"/>
-      <c r="D67" s="15"/>
-      <c r="E67" s="15"/>
-      <c r="F67" s="15"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C67" s="16"/>
+      <c r="D67" s="16"/>
+      <c r="E67" s="16"/>
+      <c r="F67" s="16"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="6">
         <v>2</v>
       </c>
-      <c r="B68" s="15" t="s">
+      <c r="B68" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C68" s="15"/>
-      <c r="D68" s="15"/>
-      <c r="E68" s="15"/>
-      <c r="F68" s="15"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C68" s="16"/>
+      <c r="D68" s="16"/>
+      <c r="E68" s="16"/>
+      <c r="F68" s="16"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="6">
         <v>3</v>
       </c>
-      <c r="B69" s="15" t="s">
+      <c r="B69" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C69" s="15"/>
-      <c r="D69" s="15"/>
-      <c r="E69" s="15"/>
-      <c r="F69" s="15"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C69" s="16"/>
+      <c r="D69" s="16"/>
+      <c r="E69" s="16"/>
+      <c r="F69" s="16"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="6">
         <v>4</v>
       </c>
-      <c r="B70" s="15" t="s">
+      <c r="B70" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C70" s="15"/>
-      <c r="D70" s="15"/>
-      <c r="E70" s="15"/>
-      <c r="F70" s="15"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C70" s="16"/>
+      <c r="D70" s="16"/>
+      <c r="E70" s="16"/>
+      <c r="F70" s="16"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>0</v>
       </c>
@@ -1539,7 +1545,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="8" t="s">
         <v>26</v>
@@ -1553,7 +1559,7 @@
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="6">
         <v>1</v>
       </c>
@@ -1571,7 +1577,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="6">
         <v>2</v>
       </c>
@@ -1589,7 +1595,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="6">
         <v>3</v>
       </c>
@@ -1607,7 +1613,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="6">
         <v>4</v>
       </c>
@@ -1625,7 +1631,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="6">
         <v>5</v>
       </c>
@@ -1642,7 +1648,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="6">
         <v>6</v>
       </c>
@@ -1659,7 +1665,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -1667,7 +1673,7 @@
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -1675,19 +1681,19 @@
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B84" s="16" t="s">
+      <c r="B84" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C84" s="16"/>
-      <c r="D84" s="16"/>
-      <c r="E84" s="16"/>
-      <c r="F84" s="16"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C84" s="20"/>
+      <c r="D84" s="20"/>
+      <c r="E84" s="20"/>
+      <c r="F84" s="20"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -1695,7 +1701,7 @@
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>1</v>
       </c>
@@ -1705,31 +1711,31 @@
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="6">
         <v>1</v>
       </c>
-      <c r="B87" s="15" t="s">
+      <c r="B87" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C87" s="15"/>
-      <c r="D87" s="15"/>
-      <c r="E87" s="15"/>
-      <c r="F87" s="15"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C87" s="16"/>
+      <c r="D87" s="16"/>
+      <c r="E87" s="16"/>
+      <c r="F87" s="16"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="6">
         <v>2</v>
       </c>
-      <c r="B88" s="15" t="s">
+      <c r="B88" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C88" s="15"/>
-      <c r="D88" s="15"/>
-      <c r="E88" s="15"/>
-      <c r="F88" s="15"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C88" s="16"/>
+      <c r="D88" s="16"/>
+      <c r="E88" s="16"/>
+      <c r="F88" s="16"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -1737,7 +1743,7 @@
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>0</v>
       </c>
@@ -1751,45 +1757,45 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="1"/>
       <c r="B91" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C91" s="18"/>
+      <c r="C91" s="19"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="6">
         <v>1</v>
       </c>
       <c r="B92" s="17">
         <v>1</v>
       </c>
-      <c r="C92" s="18"/>
+      <c r="C92" s="19"/>
       <c r="D92" s="14"/>
       <c r="E92" s="1"/>
       <c r="F92" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="6">
         <v>2</v>
       </c>
       <c r="B93" s="17">
         <v>0</v>
       </c>
-      <c r="C93" s="18"/>
+      <c r="C93" s="19"/>
       <c r="D93" s="14"/>
       <c r="E93" s="1"/>
       <c r="F93" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -1797,7 +1803,7 @@
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -1805,19 +1811,19 @@
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B96" s="16" t="s">
+      <c r="B96" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="C96" s="16"/>
-      <c r="D96" s="16"/>
-      <c r="E96" s="16"/>
-      <c r="F96" s="16"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C96" s="20"/>
+      <c r="D96" s="20"/>
+      <c r="E96" s="20"/>
+      <c r="F96" s="20"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -1825,7 +1831,7 @@
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>1</v>
       </c>
@@ -1835,82 +1841,86 @@
       <c r="E98" s="2"/>
       <c r="F98" s="2"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="6">
         <v>1</v>
       </c>
-      <c r="B99" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="C99" s="15"/>
-      <c r="D99" s="15"/>
-      <c r="E99" s="15"/>
-      <c r="F99" s="15"/>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B99" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C99" s="16"/>
+      <c r="D99" s="16"/>
+      <c r="E99" s="16"/>
+      <c r="F99" s="16"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="6">
         <v>2</v>
       </c>
-      <c r="B100" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C100" s="15"/>
-      <c r="D100" s="15"/>
-      <c r="E100" s="15"/>
-      <c r="F100" s="15"/>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="6">
+      <c r="B100" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C100" s="16"/>
+      <c r="D100" s="16"/>
+      <c r="E100" s="16"/>
+      <c r="F100" s="16"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
+      <c r="D101" s="1"/>
+      <c r="E101" s="1"/>
+      <c r="F101" s="1"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B102" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B101" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C101" s="15"/>
-      <c r="D101" s="15"/>
-      <c r="E101" s="15"/>
-      <c r="F101" s="15"/>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="1"/>
-      <c r="B102" s="1"/>
-      <c r="C102" s="1"/>
+      <c r="C102" s="13"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
-      <c r="F102" s="1"/>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B103" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C103" s="13"/>
+      <c r="F102" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103" s="1"/>
+      <c r="B103" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C103" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
-      <c r="F103" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="1"/>
-      <c r="B104" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C104" s="8" t="s">
-        <v>43</v>
+      <c r="F103" s="1"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A104" s="6">
+        <v>1</v>
+      </c>
+      <c r="B104" s="9">
+        <v>1</v>
+      </c>
+      <c r="C104" s="7">
+        <v>1</v>
       </c>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
-      <c r="F104" s="1"/>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F104" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B105" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C105" s="7">
         <v>1</v>
@@ -1918,58 +1928,38 @@
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
       <c r="F105" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="6">
-        <v>2</v>
-      </c>
-      <c r="B106" s="9">
-        <v>0</v>
-      </c>
-      <c r="C106" s="7">
-        <v>1</v>
-      </c>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
+      <c r="C106" s="1"/>
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
-      <c r="F106" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="6">
-        <v>3</v>
-      </c>
-      <c r="B107" s="7">
-        <v>1</v>
-      </c>
-      <c r="C107" s="9">
-        <v>1</v>
-      </c>
+      <c r="F106" s="1"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
+      <c r="C107" s="1"/>
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
-      <c r="F107" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="6">
-        <v>4</v>
-      </c>
-      <c r="B108" s="7">
-        <v>1</v>
-      </c>
-      <c r="C108" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D108" s="1"/>
-      <c r="E108" s="1"/>
-      <c r="F108" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F107" s="1"/>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A108" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B108" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C108" s="20"/>
+      <c r="D108" s="20"/>
+      <c r="E108" s="20"/>
+      <c r="F108" s="20"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -1977,180 +1967,185 @@
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" s="1"/>
-      <c r="B110" s="1"/>
-      <c r="C110" s="1"/>
-      <c r="D110" s="1"/>
-      <c r="E110" s="1"/>
-      <c r="F110" s="1"/>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
-        <v>2</v>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A110" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B110" s="2"/>
+      <c r="C110" s="2"/>
+      <c r="D110" s="2"/>
+      <c r="E110" s="2"/>
+      <c r="F110" s="2"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A111" s="6">
+        <v>1</v>
       </c>
       <c r="B111" s="16" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C111" s="16"/>
       <c r="D111" s="16"/>
       <c r="E111" s="16"/>
       <c r="F111" s="16"/>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112" s="1"/>
-      <c r="B112" s="1"/>
-      <c r="C112" s="1"/>
-      <c r="D112" s="1"/>
-      <c r="E112" s="1"/>
-      <c r="F112" s="1"/>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B113" s="2"/>
-      <c r="C113" s="2"/>
-      <c r="D113" s="2"/>
-      <c r="E113" s="2"/>
-      <c r="F113" s="2"/>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="6">
-        <v>1</v>
-      </c>
-      <c r="B114" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="C114" s="15"/>
-      <c r="D114" s="15"/>
-      <c r="E114" s="15"/>
-      <c r="F114" s="15"/>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" s="6">
-        <v>2</v>
-      </c>
-      <c r="B115" s="15" t="s">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A112" s="6">
+        <v>2</v>
+      </c>
+      <c r="B112" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C115" s="15"/>
-      <c r="D115" s="15"/>
-      <c r="E115" s="15"/>
-      <c r="F115" s="15"/>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="6">
+      <c r="C112" s="16"/>
+      <c r="D112" s="16"/>
+      <c r="E112" s="16"/>
+      <c r="F112" s="16"/>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A113" s="6">
         <v>3</v>
       </c>
-      <c r="B116" s="15" t="s">
+      <c r="B113" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C116" s="15"/>
-      <c r="D116" s="15"/>
-      <c r="E116" s="15"/>
-      <c r="F116" s="15"/>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" s="1"/>
-      <c r="B117" s="1"/>
-      <c r="C117" s="1"/>
+      <c r="C113" s="16"/>
+      <c r="D113" s="16"/>
+      <c r="E113" s="16"/>
+      <c r="F113" s="16"/>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
+      <c r="C114" s="1"/>
+      <c r="D114" s="1"/>
+      <c r="E114" s="1"/>
+      <c r="F114" s="1"/>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A115" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B115" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C115" s="13"/>
+      <c r="D115" s="1"/>
+      <c r="E115" s="1"/>
+      <c r="F115" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A116" s="1"/>
+      <c r="B116" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C116" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D116" s="1"/>
+      <c r="E116" s="1"/>
+      <c r="F116" s="1"/>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A117" s="6">
+        <v>1</v>
+      </c>
+      <c r="B117" s="9">
+        <v>1</v>
+      </c>
+      <c r="C117" s="7">
+        <v>1</v>
+      </c>
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
-      <c r="F117" s="1"/>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
+      <c r="F117" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A118" s="6">
+        <v>2</v>
+      </c>
+      <c r="B118" s="9">
         <v>0</v>
       </c>
-      <c r="B118" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C118" s="13"/>
+      <c r="C118" s="7">
+        <v>1</v>
+      </c>
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
-      <c r="F118" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" s="1"/>
-      <c r="B119" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C119" s="8" t="s">
-        <v>43</v>
+      <c r="F118" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A119" s="6">
+        <v>3</v>
+      </c>
+      <c r="B119" s="7">
+        <v>1</v>
+      </c>
+      <c r="C119" s="9">
+        <v>1</v>
       </c>
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
-      <c r="F119" s="1"/>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F119" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" s="6">
-        <v>1</v>
-      </c>
-      <c r="B120" s="9">
-        <v>1</v>
-      </c>
-      <c r="C120" s="7">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="B120" s="7">
+        <v>1</v>
+      </c>
+      <c r="C120" s="9" t="s">
+        <v>22</v>
       </c>
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
       <c r="F120" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="6">
-        <v>2</v>
-      </c>
-      <c r="B121" s="9">
-        <v>0</v>
-      </c>
-      <c r="C121" s="7">
-        <v>1</v>
-      </c>
-      <c r="D121" s="1"/>
-      <c r="E121" s="1"/>
-      <c r="F121" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" s="6">
-        <v>3</v>
-      </c>
-      <c r="B122" s="7">
-        <v>1</v>
-      </c>
-      <c r="C122" s="9">
-        <v>1</v>
-      </c>
-      <c r="D122" s="1"/>
-      <c r="E122" s="1"/>
-      <c r="F122" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A123" s="6">
-        <v>4</v>
-      </c>
-      <c r="B123" s="7">
-        <v>1</v>
-      </c>
-      <c r="C123" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D123" s="1"/>
-      <c r="E123" s="1"/>
-      <c r="F123" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="50">
+  <mergeCells count="49">
+    <mergeCell ref="B111:F111"/>
+    <mergeCell ref="B112:F112"/>
+    <mergeCell ref="B113:F113"/>
+    <mergeCell ref="B96:F96"/>
+    <mergeCell ref="B99:F99"/>
+    <mergeCell ref="B100:F100"/>
+    <mergeCell ref="B108:F108"/>
+    <mergeCell ref="B84:F84"/>
+    <mergeCell ref="B88:F88"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="B64:F64"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B87:F87"/>
+    <mergeCell ref="B67:F67"/>
+    <mergeCell ref="B68:F68"/>
+    <mergeCell ref="B69:F69"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B43:D43"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="B8:D8"/>
@@ -2167,40 +2162,6 @@
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B30:D30"/>
     <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B87:F87"/>
-    <mergeCell ref="B67:F67"/>
-    <mergeCell ref="B68:F68"/>
-    <mergeCell ref="B69:F69"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B50:F50"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="B52:F52"/>
-    <mergeCell ref="B64:F64"/>
-    <mergeCell ref="B84:F84"/>
-    <mergeCell ref="B88:F88"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="B93:C93"/>
-    <mergeCell ref="B114:F114"/>
-    <mergeCell ref="B115:F115"/>
-    <mergeCell ref="B116:F116"/>
-    <mergeCell ref="B96:F96"/>
-    <mergeCell ref="B99:F99"/>
-    <mergeCell ref="B100:F100"/>
-    <mergeCell ref="B101:F101"/>
-    <mergeCell ref="B111:F111"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update tabelas e testes
</commit_message>
<xml_diff>
--- a/Tabelas BVA.xlsx
+++ b/Tabelas BVA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vieir\Documents\GitHub\ESII--TP2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F92A6DE1-25B6-4196-BAF4-F503834B1A05}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA061E8C-A008-4791-A422-9A6AA68385F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10392" xr2:uid="{5BC89611-3435-46D4-BA42-03AA10355231}"/>
   </bookViews>
@@ -381,22 +381,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -753,13 +753,13 @@
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
       <c r="G1" s="10"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -780,26 +780,26 @@
       <c r="A4" s="6">
         <v>1</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
       <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>2</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
       <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -809,11 +809,11 @@
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
       <c r="E7" s="10"/>
       <c r="F7" s="3" t="s">
         <v>4</v>
@@ -824,8 +824,8 @@
       <c r="B8" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="18"/>
       <c r="E8" s="10"/>
       <c r="G8" s="10"/>
     </row>
@@ -836,8 +836,8 @@
       <c r="B9" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="18"/>
       <c r="E9" s="10"/>
       <c r="F9" s="4" t="s">
         <v>12</v>
@@ -851,8 +851,8 @@
       <c r="B10" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="18"/>
       <c r="E10" s="10"/>
       <c r="F10" s="4" t="s">
         <v>13</v>
@@ -867,13 +867,13 @@
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
@@ -889,25 +889,25 @@
       <c r="A15" s="6">
         <v>1</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>2</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
       <c r="G16" s="10"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -917,11 +917,11 @@
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
       <c r="E18" s="10"/>
       <c r="F18" s="3" t="s">
         <v>4</v>
@@ -932,8 +932,8 @@
       <c r="B19" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="18"/>
       <c r="E19" s="10"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -943,8 +943,8 @@
       <c r="B20" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="18"/>
       <c r="E20" s="10"/>
       <c r="F20" s="4" t="s">
         <v>5</v>
@@ -958,8 +958,8 @@
       <c r="B21" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="18"/>
       <c r="E21" s="10"/>
       <c r="F21" s="4" t="s">
         <v>22</v>
@@ -973,13 +973,13 @@
       <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
       <c r="G23" s="10"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -1006,26 +1006,26 @@
       <c r="A26" s="6">
         <v>1</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
       <c r="G26" s="10"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>2</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
       <c r="G27" s="10"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1057,8 +1057,8 @@
       <c r="B30" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="18"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="10"/>
@@ -1070,8 +1070,8 @@
       <c r="B31" s="17">
         <v>1</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="18"/>
       <c r="E31" s="14"/>
       <c r="F31" s="4" t="s">
         <v>6</v>
@@ -1085,8 +1085,8 @@
       <c r="B32" s="17">
         <v>0</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="18"/>
       <c r="E32" s="14"/>
       <c r="F32" s="4" t="s">
         <v>22</v>
@@ -1105,13 +1105,13 @@
       <c r="A34" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
@@ -1135,25 +1135,25 @@
       <c r="A37" s="6">
         <v>1</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
         <v>2</v>
       </c>
-      <c r="B38" s="16" t="s">
+      <c r="B38" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
@@ -1182,8 +1182,8 @@
       <c r="B41" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C41" s="18"/>
-      <c r="D41" s="19"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="18"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
     </row>
@@ -1194,8 +1194,8 @@
       <c r="B42" s="17">
         <v>1</v>
       </c>
-      <c r="C42" s="18"/>
-      <c r="D42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="18"/>
       <c r="E42" s="14"/>
       <c r="F42" s="4" t="s">
         <v>30</v>
@@ -1208,8 +1208,8 @@
       <c r="B43" s="17">
         <v>0</v>
       </c>
-      <c r="C43" s="18"/>
-      <c r="D43" s="19"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="18"/>
       <c r="E43" s="14"/>
       <c r="F43" s="4">
         <v>-1</v>
@@ -1219,13 +1219,13 @@
       <c r="A46" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="20" t="s">
+      <c r="B46" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
@@ -1249,49 +1249,49 @@
       <c r="A49" s="6">
         <v>1</v>
       </c>
-      <c r="B49" s="16" t="s">
+      <c r="B49" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C49" s="16"/>
-      <c r="D49" s="16"/>
-      <c r="E49" s="16"/>
-      <c r="F49" s="16"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="15"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="6">
         <v>2</v>
       </c>
-      <c r="B50" s="16" t="s">
+      <c r="B50" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C50" s="16"/>
-      <c r="D50" s="16"/>
-      <c r="E50" s="16"/>
-      <c r="F50" s="16"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="6">
         <v>3</v>
       </c>
-      <c r="B51" s="16" t="s">
+      <c r="B51" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C51" s="16"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="16"/>
-      <c r="F51" s="16"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="6">
         <v>4</v>
       </c>
-      <c r="B52" s="16" t="s">
+      <c r="B52" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C52" s="16"/>
-      <c r="D52" s="16"/>
-      <c r="E52" s="16"/>
-      <c r="F52" s="16"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="15"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
@@ -1457,13 +1457,13 @@
       <c r="A64" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B64" s="20" t="s">
+      <c r="B64" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C64" s="20"/>
-      <c r="D64" s="20"/>
-      <c r="E64" s="20"/>
-      <c r="F64" s="20"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="16"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
@@ -1487,49 +1487,49 @@
       <c r="A67" s="6">
         <v>1</v>
       </c>
-      <c r="B67" s="16" t="s">
+      <c r="B67" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C67" s="16"/>
-      <c r="D67" s="16"/>
-      <c r="E67" s="16"/>
-      <c r="F67" s="16"/>
+      <c r="C67" s="15"/>
+      <c r="D67" s="15"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="15"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="6">
         <v>2</v>
       </c>
-      <c r="B68" s="16" t="s">
+      <c r="B68" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C68" s="16"/>
-      <c r="D68" s="16"/>
-      <c r="E68" s="16"/>
-      <c r="F68" s="16"/>
+      <c r="C68" s="15"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="15"/>
+      <c r="F68" s="15"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="6">
         <v>3</v>
       </c>
-      <c r="B69" s="16" t="s">
+      <c r="B69" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C69" s="16"/>
-      <c r="D69" s="16"/>
-      <c r="E69" s="16"/>
-      <c r="F69" s="16"/>
+      <c r="C69" s="15"/>
+      <c r="D69" s="15"/>
+      <c r="E69" s="15"/>
+      <c r="F69" s="15"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="6">
         <v>4</v>
       </c>
-      <c r="B70" s="16" t="s">
+      <c r="B70" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C70" s="16"/>
-      <c r="D70" s="16"/>
-      <c r="E70" s="16"/>
-      <c r="F70" s="16"/>
+      <c r="C70" s="15"/>
+      <c r="D70" s="15"/>
+      <c r="E70" s="15"/>
+      <c r="F70" s="15"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
@@ -1685,13 +1685,13 @@
       <c r="A84" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B84" s="20" t="s">
+      <c r="B84" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C84" s="20"/>
-      <c r="D84" s="20"/>
-      <c r="E84" s="20"/>
-      <c r="F84" s="20"/>
+      <c r="C84" s="16"/>
+      <c r="D84" s="16"/>
+      <c r="E84" s="16"/>
+      <c r="F84" s="16"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
@@ -1715,25 +1715,25 @@
       <c r="A87" s="6">
         <v>1</v>
       </c>
-      <c r="B87" s="16" t="s">
+      <c r="B87" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C87" s="16"/>
-      <c r="D87" s="16"/>
-      <c r="E87" s="16"/>
-      <c r="F87" s="16"/>
+      <c r="C87" s="15"/>
+      <c r="D87" s="15"/>
+      <c r="E87" s="15"/>
+      <c r="F87" s="15"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="6">
         <v>2</v>
       </c>
-      <c r="B88" s="16" t="s">
+      <c r="B88" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C88" s="16"/>
-      <c r="D88" s="16"/>
-      <c r="E88" s="16"/>
-      <c r="F88" s="16"/>
+      <c r="C88" s="15"/>
+      <c r="D88" s="15"/>
+      <c r="E88" s="15"/>
+      <c r="F88" s="15"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
@@ -1762,7 +1762,7 @@
       <c r="B91" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C91" s="19"/>
+      <c r="C91" s="18"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
@@ -1774,7 +1774,7 @@
       <c r="B92" s="17">
         <v>1</v>
       </c>
-      <c r="C92" s="19"/>
+      <c r="C92" s="18"/>
       <c r="D92" s="14"/>
       <c r="E92" s="1"/>
       <c r="F92" s="4" t="s">
@@ -1788,7 +1788,7 @@
       <c r="B93" s="17">
         <v>0</v>
       </c>
-      <c r="C93" s="19"/>
+      <c r="C93" s="18"/>
       <c r="D93" s="14"/>
       <c r="E93" s="1"/>
       <c r="F93" s="4" t="s">
@@ -1815,13 +1815,13 @@
       <c r="A96" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B96" s="20" t="s">
+      <c r="B96" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C96" s="20"/>
-      <c r="D96" s="20"/>
-      <c r="E96" s="20"/>
-      <c r="F96" s="20"/>
+      <c r="C96" s="16"/>
+      <c r="D96" s="16"/>
+      <c r="E96" s="16"/>
+      <c r="F96" s="16"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="1"/>
@@ -1845,25 +1845,25 @@
       <c r="A99" s="6">
         <v>1</v>
       </c>
-      <c r="B99" s="16" t="s">
+      <c r="B99" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="C99" s="16"/>
-      <c r="D99" s="16"/>
-      <c r="E99" s="16"/>
-      <c r="F99" s="16"/>
+      <c r="C99" s="15"/>
+      <c r="D99" s="15"/>
+      <c r="E99" s="15"/>
+      <c r="F99" s="15"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="6">
         <v>2</v>
       </c>
-      <c r="B100" s="16" t="s">
+      <c r="B100" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C100" s="16"/>
-      <c r="D100" s="16"/>
-      <c r="E100" s="16"/>
-      <c r="F100" s="16"/>
+      <c r="C100" s="15"/>
+      <c r="D100" s="15"/>
+      <c r="E100" s="15"/>
+      <c r="F100" s="15"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" s="1"/>
@@ -1951,13 +1951,13 @@
       <c r="A108" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B108" s="20" t="s">
+      <c r="B108" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C108" s="20"/>
-      <c r="D108" s="20"/>
-      <c r="E108" s="20"/>
-      <c r="F108" s="20"/>
+      <c r="C108" s="16"/>
+      <c r="D108" s="16"/>
+      <c r="E108" s="16"/>
+      <c r="F108" s="16"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" s="1"/>
@@ -1981,37 +1981,37 @@
       <c r="A111" s="6">
         <v>1</v>
       </c>
-      <c r="B111" s="16" t="s">
+      <c r="B111" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C111" s="16"/>
-      <c r="D111" s="16"/>
-      <c r="E111" s="16"/>
-      <c r="F111" s="16"/>
+      <c r="C111" s="15"/>
+      <c r="D111" s="15"/>
+      <c r="E111" s="15"/>
+      <c r="F111" s="15"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" s="6">
         <v>2</v>
       </c>
-      <c r="B112" s="16" t="s">
+      <c r="B112" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C112" s="16"/>
-      <c r="D112" s="16"/>
-      <c r="E112" s="16"/>
-      <c r="F112" s="16"/>
+      <c r="C112" s="15"/>
+      <c r="D112" s="15"/>
+      <c r="E112" s="15"/>
+      <c r="F112" s="15"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" s="6">
         <v>3</v>
       </c>
-      <c r="B113" s="16" t="s">
+      <c r="B113" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C113" s="16"/>
-      <c r="D113" s="16"/>
-      <c r="E113" s="16"/>
-      <c r="F113" s="16"/>
+      <c r="C113" s="15"/>
+      <c r="D113" s="15"/>
+      <c r="E113" s="15"/>
+      <c r="F113" s="15"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" s="1"/>
@@ -2113,23 +2113,22 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="B111:F111"/>
-    <mergeCell ref="B112:F112"/>
-    <mergeCell ref="B113:F113"/>
-    <mergeCell ref="B96:F96"/>
-    <mergeCell ref="B99:F99"/>
-    <mergeCell ref="B100:F100"/>
-    <mergeCell ref="B108:F108"/>
-    <mergeCell ref="B84:F84"/>
-    <mergeCell ref="B88:F88"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="B93:C93"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B50:F50"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="B52:F52"/>
-    <mergeCell ref="B64:F64"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B26:F26"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B15:F15"/>
@@ -2146,22 +2145,23 @@
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="B42:D42"/>
     <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="B64:F64"/>
+    <mergeCell ref="B84:F84"/>
+    <mergeCell ref="B88:F88"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="B111:F111"/>
+    <mergeCell ref="B112:F112"/>
+    <mergeCell ref="B113:F113"/>
+    <mergeCell ref="B96:F96"/>
+    <mergeCell ref="B99:F99"/>
+    <mergeCell ref="B100:F100"/>
+    <mergeCell ref="B108:F108"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>